<commit_message>
feat: save_excel 데이터 형식 변경
</commit_message>
<xml_diff>
--- a/item_info2.xlsx
+++ b/item_info2.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -637,10 +637,8 @@
           <t>https://www.grandviewresearch.com/industry-analysis/router-market-report</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>18070000000</t>
-        </is>
+      <c r="N4" t="n">
+        <v>18070000000</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -699,10 +697,8 @@
           <t>https://www.statista.com/forecasts/1149791/laptops-revenue-worldwide</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>208700000000</t>
-        </is>
+      <c r="N5" t="n">
+        <v>208700000000</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -1059,62 +1055,62 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>900,500,000</t>
+          <t>460000000(추정)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://www.statista.com/outlook/dmo/ecommerce/electronics/audio-video-equipment/headphones/south-korea</t>
+          <t>[1]에 따르면 2022년 한국 무선 헤드폰 시장이 급격히 성장했으나, 전체 헤드셋 시장규모 공식 집계 데이터는 없음. 30만원 이상 프리미엄 무선 헤드폰 집중 성장, 주요 브랜드 소매가/점유율 및 글로벌 대비 로컬 소비 추세를 감안하여 400억~500억원대 규모로 추산.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>947,800,000</t>
+          <t>550000000(추정)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://www.statista.com/outlook/dmo/ecommerce/electronics/audio-video-equipment/headphones/south-korea</t>
+          <t>[1]의 성장률 인용 및 프리미엄 헤드폰 시장 확대 전망을 토대로 약 20% 이상 성장 반영, 대략 550억원 수준으로 추산.</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>991,200,000</t>
+          <t>650000000(추정)</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://www.statista.com/outlook/dmo/ecommerce/electronics/audio-video-equipment/headphones/south-korea</t>
+          <t>[1]의 '올해도 시장 확대 전망'과 글로벌 이어폰·헤드폰 동종 CAGR을 적용해 약 18% 추가 성장 반영. 합리적 예측치로 약 650억원으로 산출.</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>72,580,000,000</t>
+          <t>34300000000(추정)</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>https://www.fortunebusinessinsights.com/headset-market-102570</t>
+          <t>[3] 글로벌 이어폰 및 헤드폰 시장은 약 $343억 (34,300,000,000) 달러로 제시. 별도의 헤드셋 단독 데이터는 없으나 유사제품군이므로 전체 규모 활용.</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>81,330,000,000</t>
+          <t>35000000000(추정)</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>https://www.fortunebusinessinsights.com/headset-market-102570</t>
+          <t>[3] 자주 묻는 질문 섹션에서 글로벌 이어폰·헤드폰 시장이 $350억 달러로 상승했다고 명시되어 있음.</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>86,150,000,000</t>
+          <t>34000000000</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>https://www.mordorintelligence.com/industry-reports/headsets-market</t>
+          <t>[3]에서 '글로벌 이어폰과 헤드폰 시장 규모는 340억 달러'라고 구체적으로 언급됨.</t>
         </is>
       </c>
       <c r="P17" t="inlineStr"/>

</xml_diff>